<commit_message>
Blade of Heaven Steel
</commit_message>
<xml_diff>
--- a/BetterNames-v2.2-Weapons.xlsx
+++ b/BetterNames-v2.2-Weapons.xlsx
@@ -10756,9 +10756,6 @@
     <t>Short Jinkblade of Wounds</t>
   </si>
   <si>
-    <t>Short Steel Blade of Heaven</t>
-  </si>
-  <si>
     <t>Short Fireblade</t>
   </si>
   <si>
@@ -11117,6 +11114,9 @@
   </si>
   <si>
     <t>Short Dagger Blindng Acrobatics</t>
+  </si>
+  <si>
+    <t>Short Blade of Heaven Steel</t>
   </si>
 </sst>
 </file>
@@ -11959,8 +11959,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J636"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F636"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12152,7 +12152,7 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -12184,7 +12184,7 @@
         <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -12344,7 +12344,7 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -12504,7 +12504,7 @@
         <v>10000</v>
       </c>
       <c r="F17" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -12568,7 +12568,7 @@
         <v>80</v>
       </c>
       <c r="F19" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -13304,7 +13304,7 @@
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
@@ -14136,7 +14136,7 @@
         <v>20000</v>
       </c>
       <c r="F68" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="G68">
         <f t="shared" si="2"/>
@@ -14584,7 +14584,7 @@
         <v>300</v>
       </c>
       <c r="F82" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="G82">
         <f t="shared" si="2"/>
@@ -15608,7 +15608,7 @@
         <v>120</v>
       </c>
       <c r="F114" t="s">
-        <v>3576</v>
+        <v>3696</v>
       </c>
       <c r="G114">
         <f t="shared" si="2"/>
@@ -15989,7 +15989,7 @@
         <v>25</v>
       </c>
       <c r="F126" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="G126">
         <f t="shared" si="2"/>
@@ -17257,7 +17257,7 @@
         <v>15</v>
       </c>
       <c r="F166" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="G166">
         <f t="shared" si="4"/>
@@ -17289,7 +17289,7 @@
         <v>15</v>
       </c>
       <c r="F167" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="G167">
         <f t="shared" si="4"/>
@@ -17321,7 +17321,7 @@
         <v>15</v>
       </c>
       <c r="F168" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="G168">
         <f t="shared" si="4"/>
@@ -17353,7 +17353,7 @@
         <v>15</v>
       </c>
       <c r="F169" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="G169">
         <f t="shared" si="4"/>
@@ -17385,7 +17385,7 @@
         <v>60</v>
       </c>
       <c r="F170" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="G170">
         <f t="shared" si="4"/>
@@ -17417,7 +17417,7 @@
         <v>60</v>
       </c>
       <c r="F171" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="G171">
         <f t="shared" si="4"/>
@@ -17449,7 +17449,7 @@
         <v>65</v>
       </c>
       <c r="F172" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="G172">
         <f t="shared" si="4"/>
@@ -17481,7 +17481,7 @@
         <v>60</v>
       </c>
       <c r="F173" t="s">
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="G173">
         <f t="shared" si="4"/>
@@ -17705,7 +17705,7 @@
         <v>40</v>
       </c>
       <c r="F180" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="G180">
         <f t="shared" si="4"/>
@@ -17737,7 +17737,7 @@
         <v>35</v>
       </c>
       <c r="F181" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="G181">
         <f t="shared" si="4"/>
@@ -17769,7 +17769,7 @@
         <v>35</v>
       </c>
       <c r="F182" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="G182">
         <f t="shared" si="4"/>
@@ -17801,7 +17801,7 @@
         <v>35</v>
       </c>
       <c r="F183" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="G183">
         <f t="shared" si="4"/>
@@ -18793,7 +18793,7 @@
         <v>17</v>
       </c>
       <c r="F214" s="3" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="G214">
         <f t="shared" si="6"/>
@@ -19654,7 +19654,7 @@
         <v>17</v>
       </c>
       <c r="F241" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="G241">
         <f t="shared" si="6"/>
@@ -19686,7 +19686,7 @@
         <v>17</v>
       </c>
       <c r="F242" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="G242">
         <f t="shared" si="6"/>
@@ -19718,7 +19718,7 @@
         <v>17</v>
       </c>
       <c r="F243" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="G243">
         <f t="shared" si="6"/>
@@ -19750,7 +19750,7 @@
         <v>17</v>
       </c>
       <c r="F244" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="G244">
         <f t="shared" si="6"/>
@@ -19782,7 +19782,7 @@
         <v>65</v>
       </c>
       <c r="F245" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="G245">
         <f t="shared" si="6"/>
@@ -19814,7 +19814,7 @@
         <v>65</v>
       </c>
       <c r="F246" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="G246">
         <f t="shared" si="6"/>
@@ -19846,7 +19846,7 @@
         <v>65</v>
       </c>
       <c r="F247" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
       <c r="G247">
         <f t="shared" si="6"/>
@@ -19878,7 +19878,7 @@
         <v>70</v>
       </c>
       <c r="F248" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="G248">
         <f t="shared" si="6"/>
@@ -19974,7 +19974,7 @@
         <v>55</v>
       </c>
       <c r="F251" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="G251">
         <f t="shared" si="6"/>
@@ -20006,7 +20006,7 @@
         <v>55</v>
       </c>
       <c r="F252" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="G252">
         <f t="shared" si="6"/>
@@ -20038,7 +20038,7 @@
         <v>55</v>
       </c>
       <c r="F253" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="G253">
         <f t="shared" si="6"/>
@@ -20070,7 +20070,7 @@
         <v>55</v>
       </c>
       <c r="F254" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="G254">
         <f t="shared" si="6"/>
@@ -21696,7 +21696,7 @@
         <v>4100</v>
       </c>
       <c r="F305" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="G305">
         <f t="shared" si="8"/>
@@ -21728,7 +21728,7 @@
         <v>4100</v>
       </c>
       <c r="F306" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="G306">
         <f t="shared" si="8"/>
@@ -21760,7 +21760,7 @@
         <v>4100</v>
       </c>
       <c r="F307" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="G307">
         <f t="shared" si="8"/>
@@ -21792,7 +21792,7 @@
         <v>4100</v>
       </c>
       <c r="F308" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="G308">
         <f t="shared" si="8"/>
@@ -21824,7 +21824,7 @@
         <v>350</v>
       </c>
       <c r="F309" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="G309">
         <f t="shared" si="8"/>
@@ -21856,7 +21856,7 @@
         <v>350</v>
       </c>
       <c r="F310" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
       <c r="G310">
         <f t="shared" si="8"/>
@@ -21888,7 +21888,7 @@
         <v>350</v>
       </c>
       <c r="F311" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="G311">
         <f t="shared" si="8"/>
@@ -21920,7 +21920,7 @@
         <v>350</v>
       </c>
       <c r="F312" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
       <c r="G312">
         <f t="shared" si="8"/>
@@ -22144,7 +22144,7 @@
         <v>120</v>
       </c>
       <c r="F319" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="G319">
         <f t="shared" si="8"/>
@@ -22176,7 +22176,7 @@
         <v>120</v>
       </c>
       <c r="F320" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="G320">
         <f t="shared" si="8"/>
@@ -22208,7 +22208,7 @@
         <v>120</v>
       </c>
       <c r="F321" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="G321">
         <f t="shared" ref="G321:G384" si="10">LEN(F321)</f>
@@ -22240,7 +22240,7 @@
         <v>120</v>
       </c>
       <c r="F322" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="G322">
         <f t="shared" si="10"/>
@@ -24389,7 +24389,7 @@
         <v>5000</v>
       </c>
       <c r="F390" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="G390">
         <f t="shared" si="12"/>
@@ -26052,7 +26052,7 @@
         <v>55</v>
       </c>
       <c r="F443" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
       <c r="G443">
         <f t="shared" si="14"/>
@@ -26084,7 +26084,7 @@
         <v>45</v>
       </c>
       <c r="F444" s="3" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="G444">
         <f t="shared" si="14"/>
@@ -27346,7 +27346,7 @@
         <v>11000</v>
       </c>
       <c r="F484" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="G484">
         <f t="shared" si="14"/>
@@ -28108,7 +28108,7 @@
         <v>1000</v>
       </c>
       <c r="F508" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="G508">
         <f t="shared" si="16"/>
@@ -29225,7 +29225,7 @@
         <v>1000</v>
       </c>
       <c r="F543" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="G543">
         <f t="shared" si="16"/>
@@ -29507,7 +29507,7 @@
         <v>30</v>
       </c>
       <c r="F552" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="G552">
         <f t="shared" si="16"/>
@@ -43100,7 +43100,7 @@
         <v>45</v>
       </c>
       <c r="F601" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="G601">
         <f>LEN(F601)</f>
@@ -43124,7 +43124,7 @@
         <v>100</v>
       </c>
       <c r="F602" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="G602">
         <f t="shared" ref="G602:G663" si="0">LEN(F602)</f>
@@ -43148,7 +43148,7 @@
         <v>650</v>
       </c>
       <c r="F603" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="G603">
         <f t="shared" si="0"/>
@@ -43172,7 +43172,7 @@
         <v>4000</v>
       </c>
       <c r="F604" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
       <c r="G604">
         <f t="shared" si="0"/>
@@ -43532,7 +43532,7 @@
         <v>1200</v>
       </c>
       <c r="F619" t="s">
-        <v>3692</v>
+        <v>3691</v>
       </c>
       <c r="G619">
         <f t="shared" si="0"/>
@@ -43556,7 +43556,7 @@
         <v>1200</v>
       </c>
       <c r="F620" t="s">
-        <v>3693</v>
+        <v>3692</v>
       </c>
       <c r="G620">
         <f t="shared" si="0"/>
@@ -43721,7 +43721,7 @@
         <v>160</v>
       </c>
       <c r="F627" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="G627">
         <f t="shared" si="0"/>
@@ -43907,7 +43907,7 @@
         <v>200</v>
       </c>
       <c r="F635" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="G635">
         <f t="shared" si="0"/>
@@ -44105,7 +44105,7 @@
         <v>40</v>
       </c>
       <c r="F644" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="G644">
         <f t="shared" si="0"/>
@@ -44129,7 +44129,7 @@
         <v>40</v>
       </c>
       <c r="F645" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="G645">
         <f t="shared" si="0"/>
@@ -44273,7 +44273,7 @@
         <v>80</v>
       </c>
       <c r="F651" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
       <c r="G651">
         <f t="shared" si="0"/>
@@ -44297,7 +44297,7 @@
         <v>80</v>
       </c>
       <c r="F652" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
       <c r="G652">
         <f t="shared" si="0"/>
@@ -44819,7 +44819,7 @@
         <v>500</v>
       </c>
       <c r="F674" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="G674">
         <f t="shared" si="1"/>
@@ -44867,7 +44867,7 @@
         <v>1000</v>
       </c>
       <c r="F676" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="G676">
         <f t="shared" si="1"/>
@@ -45515,7 +45515,7 @@
         <v>1000</v>
       </c>
       <c r="F703" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="G703">
         <f t="shared" si="1"/>
@@ -45731,7 +45731,7 @@
         <v>1100</v>
       </c>
       <c r="F712" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
       <c r="G712">
         <f t="shared" si="1"/>
@@ -45755,7 +45755,7 @@
         <v>1200</v>
       </c>
       <c r="F713" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="G713">
         <f t="shared" si="1"/>
@@ -45875,7 +45875,7 @@
         <v>250</v>
       </c>
       <c r="F718" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="G718">
         <f t="shared" si="1"/>
@@ -46085,7 +46085,7 @@
         <v>12000</v>
       </c>
       <c r="F727" s="3" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="G727">
         <f t="shared" si="1"/>
@@ -46349,7 +46349,7 @@
         <v>150</v>
       </c>
       <c r="F738" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="G738">
         <f t="shared" si="2"/>
@@ -46493,7 +46493,7 @@
         <v>5000</v>
       </c>
       <c r="F744" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="G744">
         <f t="shared" si="2"/>
@@ -46589,7 +46589,7 @@
         <v>7000</v>
       </c>
       <c r="F748" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="G748">
         <f t="shared" si="2"/>
@@ -46613,7 +46613,7 @@
         <v>18000</v>
       </c>
       <c r="F749" s="5" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
       <c r="G749">
         <f t="shared" si="2"/>
@@ -46733,7 +46733,7 @@
         <v>4500</v>
       </c>
       <c r="F754" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="G754">
         <f t="shared" si="2"/>
@@ -46757,7 +46757,7 @@
         <v>8700</v>
       </c>
       <c r="F755" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="G755">
         <f t="shared" si="2"/>
@@ -46781,7 +46781,7 @@
         <v>120</v>
       </c>
       <c r="F756" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="G756">
         <f t="shared" si="2"/>
@@ -46946,7 +46946,7 @@
         <v>35</v>
       </c>
       <c r="F763" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="G763">
         <f t="shared" si="2"/>
@@ -47423,7 +47423,7 @@
         <v>5200</v>
       </c>
       <c r="F783" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="G783">
         <f t="shared" si="2"/>
@@ -47519,7 +47519,7 @@
         <v>35</v>
       </c>
       <c r="F787" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="G787">
         <f t="shared" si="2"/>
@@ -47591,7 +47591,7 @@
         <v>65</v>
       </c>
       <c r="F790" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="G790">
         <f t="shared" si="2"/>
@@ -47687,7 +47687,7 @@
         <v>600</v>
       </c>
       <c r="F794" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="G794">
         <f t="shared" si="3"/>
@@ -47711,7 +47711,7 @@
         <v>800</v>
       </c>
       <c r="F795" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="G795">
         <f t="shared" si="3"/>
@@ -47900,7 +47900,7 @@
         <v>55</v>
       </c>
       <c r="F803" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="G803">
         <f t="shared" si="3"/>
@@ -48089,7 +48089,7 @@
         <v>200</v>
       </c>
       <c r="F811" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="G811">
         <f t="shared" si="3"/>
@@ -48137,7 +48137,7 @@
         <v>400</v>
       </c>
       <c r="F813" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="G813">
         <f t="shared" si="3"/>
@@ -48629,7 +48629,7 @@
         <v>120</v>
       </c>
       <c r="F834" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="G834">
         <f t="shared" si="3"/>
@@ -48653,7 +48653,7 @@
         <v>60</v>
       </c>
       <c r="F835" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
       <c r="G835">
         <f t="shared" si="3"/>
@@ -48821,7 +48821,7 @@
         <v>10000</v>
       </c>
       <c r="F842" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="G842">
         <f t="shared" si="3"/>
@@ -48965,7 +48965,7 @@
         <v>80</v>
       </c>
       <c r="F848" s="3" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
       <c r="G848">
         <f t="shared" si="3"/>
@@ -49247,7 +49247,7 @@
         <v>24</v>
       </c>
       <c r="F860" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
       <c r="G860">
         <f t="shared" si="4"/>
@@ -49271,7 +49271,7 @@
         <v>10000</v>
       </c>
       <c r="F861" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
       <c r="G861">
         <f t="shared" si="4"/>
@@ -49295,7 +49295,7 @@
         <v>20</v>
       </c>
       <c r="F862" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="G862">
         <f t="shared" si="4"/>
@@ -49532,7 +49532,7 @@
         <v>24000</v>
       </c>
       <c r="F872" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="G872">
         <f t="shared" si="4"/>
@@ -49646,7 +49646,7 @@
         <v>60000</v>
       </c>
       <c r="F877" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="G877">
         <f t="shared" si="4"/>
@@ -49670,7 +49670,7 @@
         <v>10000</v>
       </c>
       <c r="F878" t="s">
-        <v>3694</v>
+        <v>3693</v>
       </c>
       <c r="G878">
         <f t="shared" si="4"/>
@@ -49742,7 +49742,7 @@
         <v>11000</v>
       </c>
       <c r="F881" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
       <c r="G881">
         <f t="shared" si="4"/>
@@ -49862,7 +49862,7 @@
         <v>40</v>
       </c>
       <c r="F886" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="G886">
         <f t="shared" si="4"/>
@@ -49910,7 +49910,7 @@
         <v>25</v>
       </c>
       <c r="F888" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="G888">
         <f t="shared" si="4"/>
@@ -50216,7 +50216,7 @@
         <v>100</v>
       </c>
       <c r="F901" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="G901">
         <f t="shared" si="4"/>
@@ -50501,7 +50501,7 @@
         <v>60</v>
       </c>
       <c r="F913" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="G913">
         <f t="shared" si="4"/>
@@ -50717,7 +50717,7 @@
         <v>800</v>
       </c>
       <c r="F922" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="G922">
         <f t="shared" si="5"/>
@@ -50741,7 +50741,7 @@
         <v>125</v>
       </c>
       <c r="F923" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
       <c r="G923">
         <f t="shared" si="5"/>
@@ -51005,7 +51005,7 @@
         <v>4600</v>
       </c>
       <c r="F934" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="G934">
         <f t="shared" si="5"/>
@@ -51029,7 +51029,7 @@
         <v>4600</v>
       </c>
       <c r="F935" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="G935">
         <f t="shared" si="5"/>
@@ -51149,7 +51149,7 @@
         <v>650</v>
       </c>
       <c r="F940" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
       <c r="G940">
         <f t="shared" si="5"/>
@@ -51197,7 +51197,7 @@
         <v>600</v>
       </c>
       <c r="F942" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
       <c r="G942">
         <f t="shared" si="5"/>
@@ -51293,7 +51293,7 @@
         <v>50000</v>
       </c>
       <c r="F946" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="G946">
         <f t="shared" si="5"/>
@@ -51317,7 +51317,7 @@
         <v>35000</v>
       </c>
       <c r="F947" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="G947">
         <f t="shared" si="5"/>
@@ -51389,7 +51389,7 @@
         <v>110</v>
       </c>
       <c r="F950" s="3" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
       <c r="G950">
         <f t="shared" si="5"/>
@@ -51509,7 +51509,7 @@
         <v>20000</v>
       </c>
       <c r="F955" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
       <c r="G955">
         <f t="shared" si="5"/>
@@ -51605,7 +51605,7 @@
         <v>18000</v>
       </c>
       <c r="F959" t="s">
-        <v>3681</v>
+        <v>3680</v>
       </c>
       <c r="G959">
         <f t="shared" si="5"/>
@@ -51653,7 +51653,7 @@
         <v>38000</v>
       </c>
       <c r="F961" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="G961">
         <f t="shared" si="5"/>
@@ -52844,7 +52844,7 @@
         <v>430</v>
       </c>
       <c r="F1012" s="2" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="G1012">
         <f t="shared" si="6"/>
@@ -53729,7 +53729,7 @@
         <v>35000</v>
       </c>
       <c r="F1049" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="G1049">
         <f t="shared" si="7"/>
@@ -54200,7 +54200,7 @@
         <v>2000</v>
       </c>
       <c r="F1069" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
       <c r="G1069">
         <f t="shared" si="8"/>
@@ -56120,7 +56120,7 @@
         <v>300</v>
       </c>
       <c r="F1162" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
       <c r="G1162">
         <f t="shared" si="9"/>
@@ -56264,7 +56264,7 @@
         <v>8000</v>
       </c>
       <c r="F1168" t="s">
-        <v>3685</v>
+        <v>3684</v>
       </c>
       <c r="G1168">
         <f t="shared" si="9"/>
@@ -56357,7 +56357,7 @@
         <v>900</v>
       </c>
       <c r="F1172" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="G1172">
         <f t="shared" si="9"/>
@@ -56474,7 +56474,7 @@
         <v>13</v>
       </c>
       <c r="F1177" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="G1177">
         <f t="shared" si="9"/>
@@ -56618,7 +56618,7 @@
         <v>500</v>
       </c>
       <c r="F1183" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="G1183">
         <f t="shared" si="10"/>
@@ -59801,7 +59801,7 @@
         <v>200</v>
       </c>
       <c r="F1316" t="s">
-        <v>3688</v>
+        <v>3687</v>
       </c>
       <c r="G1316">
         <f t="shared" si="12"/>
@@ -61814,7 +61814,7 @@
         <v>40</v>
       </c>
       <c r="F1392" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
       <c r="G1392">
         <f t="shared" si="15"/>
@@ -61920,7 +61920,7 @@
         <v>10000</v>
       </c>
       <c r="F1396" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="G1396">
         <f t="shared" si="15"/>
@@ -62480,7 +62480,7 @@
         <v>1000</v>
       </c>
       <c r="F1416" t="s">
-        <v>3690</v>
+        <v>3689</v>
       </c>
       <c r="G1416">
         <f t="shared" si="15"/>
@@ -62508,7 +62508,7 @@
         <v>165</v>
       </c>
       <c r="F1417" t="s">
-        <v>3691</v>
+        <v>3690</v>
       </c>
       <c r="G1417">
         <f t="shared" si="15"/>
@@ -62676,7 +62676,7 @@
         <v>0</v>
       </c>
       <c r="F1423" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="G1423">
         <f t="shared" si="15"/>
@@ -62986,7 +62986,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -63062,7 +63064,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -63077,7 +63079,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -63152,7 +63154,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -63227,7 +63229,7 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -63257,7 +63259,7 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -63602,7 +63604,7 @@
         <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -63992,7 +63994,7 @@
         <v>147</v>
       </c>
       <c r="C67" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="1"/>
@@ -64202,7 +64204,7 @@
         <v>175</v>
       </c>
       <c r="C81" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
@@ -64682,11 +64684,11 @@
         <v>238</v>
       </c>
       <c r="C113" t="s">
-        <v>3576</v>
+        <v>3696</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="1"/>
-        <v>{ID="steel blade of heaven", name="Short Steel Blade of Heaven"},</v>
+        <v>{ID="steel blade of heaven", name="Short Blade of Heaven Steel"},</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -64847,7 +64849,7 @@
         <v>262</v>
       </c>
       <c r="C124" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="D124" t="str">
         <f t="shared" si="1"/>
@@ -65387,7 +65389,7 @@
         <v>343</v>
       </c>
       <c r="C160" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="D160" t="str">
         <f t="shared" si="2"/>
@@ -65402,7 +65404,7 @@
         <v>345</v>
       </c>
       <c r="C161" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="D161" t="str">
         <f t="shared" si="2"/>
@@ -65417,7 +65419,7 @@
         <v>347</v>
       </c>
       <c r="C162" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="D162" t="str">
         <f t="shared" si="2"/>
@@ -65432,7 +65434,7 @@
         <v>349</v>
       </c>
       <c r="C163" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="2"/>
@@ -65447,7 +65449,7 @@
         <v>351</v>
       </c>
       <c r="C164" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="2"/>
@@ -65462,7 +65464,7 @@
         <v>353</v>
       </c>
       <c r="C165" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="D165" t="str">
         <f t="shared" si="2"/>
@@ -65477,7 +65479,7 @@
         <v>355</v>
       </c>
       <c r="C166" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="D166" t="str">
         <f t="shared" si="2"/>
@@ -65492,7 +65494,7 @@
         <v>357</v>
       </c>
       <c r="C167" t="s">
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="D167" t="str">
         <f t="shared" si="2"/>
@@ -65597,7 +65599,7 @@
         <v>371</v>
       </c>
       <c r="C174" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="D174" t="str">
         <f t="shared" si="2"/>
@@ -65612,7 +65614,7 @@
         <v>373</v>
       </c>
       <c r="C175" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="D175" t="str">
         <f t="shared" si="2"/>
@@ -65627,7 +65629,7 @@
         <v>375</v>
       </c>
       <c r="C176" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="D176" t="str">
         <f t="shared" si="2"/>
@@ -65642,7 +65644,7 @@
         <v>377</v>
       </c>
       <c r="C177" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="D177" t="str">
         <f t="shared" si="2"/>
@@ -66107,7 +66109,7 @@
         <v>439</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="D208" t="str">
         <f t="shared" si="3"/>
@@ -66497,7 +66499,7 @@
         <v>493</v>
       </c>
       <c r="C234" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="D234" t="str">
         <f t="shared" si="3"/>
@@ -66512,7 +66514,7 @@
         <v>495</v>
       </c>
       <c r="C235" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="D235" t="str">
         <f t="shared" si="3"/>
@@ -66527,7 +66529,7 @@
         <v>497</v>
       </c>
       <c r="C236" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="D236" t="str">
         <f t="shared" si="3"/>
@@ -66542,7 +66544,7 @@
         <v>499</v>
       </c>
       <c r="C237" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="D237" t="str">
         <f t="shared" si="3"/>
@@ -66557,7 +66559,7 @@
         <v>501</v>
       </c>
       <c r="C238" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="D238" t="str">
         <f t="shared" si="3"/>
@@ -66572,7 +66574,7 @@
         <v>503</v>
       </c>
       <c r="C239" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="D239" t="str">
         <f t="shared" si="3"/>
@@ -66587,7 +66589,7 @@
         <v>505</v>
       </c>
       <c r="C240" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
       <c r="D240" t="str">
         <f t="shared" si="3"/>
@@ -66602,7 +66604,7 @@
         <v>507</v>
       </c>
       <c r="C241" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="D241" t="str">
         <f t="shared" si="3"/>
@@ -66647,7 +66649,7 @@
         <v>513</v>
       </c>
       <c r="C244" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="D244" t="str">
         <f t="shared" si="3"/>
@@ -66662,7 +66664,7 @@
         <v>515</v>
       </c>
       <c r="C245" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="D245" t="str">
         <f t="shared" si="3"/>
@@ -66677,7 +66679,7 @@
         <v>517</v>
       </c>
       <c r="C246" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="D246" t="str">
         <f t="shared" si="3"/>
@@ -66692,7 +66694,7 @@
         <v>519</v>
       </c>
       <c r="C247" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="D247" t="str">
         <f t="shared" si="3"/>
@@ -67427,7 +67429,7 @@
         <v>621</v>
       </c>
       <c r="C296" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="D296" t="str">
         <f t="shared" si="4"/>
@@ -67442,7 +67444,7 @@
         <v>623</v>
       </c>
       <c r="C297" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="D297" t="str">
         <f t="shared" si="4"/>
@@ -67457,7 +67459,7 @@
         <v>625</v>
       </c>
       <c r="C298" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="D298" t="str">
         <f t="shared" si="4"/>
@@ -67472,7 +67474,7 @@
         <v>627</v>
       </c>
       <c r="C299" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="D299" t="str">
         <f t="shared" si="4"/>
@@ -67487,7 +67489,7 @@
         <v>629</v>
       </c>
       <c r="C300" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="D300" t="str">
         <f t="shared" si="4"/>
@@ -67502,7 +67504,7 @@
         <v>631</v>
       </c>
       <c r="C301" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
       <c r="D301" t="str">
         <f t="shared" si="4"/>
@@ -67517,7 +67519,7 @@
         <v>633</v>
       </c>
       <c r="C302" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="D302" t="str">
         <f t="shared" si="4"/>
@@ -67532,7 +67534,7 @@
         <v>635</v>
       </c>
       <c r="C303" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
       <c r="D303" t="str">
         <f t="shared" si="4"/>
@@ -67637,7 +67639,7 @@
         <v>649</v>
       </c>
       <c r="C310" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="D310" t="str">
         <f t="shared" si="4"/>
@@ -67652,7 +67654,7 @@
         <v>651</v>
       </c>
       <c r="C311" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="D311" t="str">
         <f t="shared" si="4"/>
@@ -67667,7 +67669,7 @@
         <v>653</v>
       </c>
       <c r="C312" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="D312" t="str">
         <f t="shared" si="4"/>
@@ -67682,7 +67684,7 @@
         <v>655</v>
       </c>
       <c r="C313" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="D313" t="str">
         <f t="shared" si="4"/>
@@ -68567,7 +68569,7 @@
         <v>38</v>
       </c>
       <c r="C372" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="D372" t="str">
         <f t="shared" si="5"/>
@@ -69197,7 +69199,7 @@
         <v>888</v>
       </c>
       <c r="C414" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
       <c r="D414" t="str">
         <f t="shared" si="6"/>
@@ -69212,7 +69214,7 @@
         <v>890</v>
       </c>
       <c r="C415" s="3" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="D415" t="str">
         <f t="shared" si="6"/>
@@ -69722,7 +69724,7 @@
         <v>950</v>
       </c>
       <c r="C449" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="D449" t="str">
         <f t="shared" si="6"/>
@@ -70052,7 +70054,7 @@
         <v>992</v>
       </c>
       <c r="C471" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="D471" t="str">
         <f t="shared" si="7"/>
@@ -70562,7 +70564,7 @@
         <v>1057</v>
       </c>
       <c r="C505" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="D505" t="str">
         <f t="shared" si="7"/>
@@ -70679,7 +70681,7 @@
         <v>1075</v>
       </c>
       <c r="C513" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="D513" t="str">
         <f t="shared" si="7"/>
@@ -71909,7 +71911,7 @@
         <v>1367</v>
       </c>
       <c r="C595" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="D595" s="2" t="str">
         <f t="shared" si="9"/>
@@ -71924,7 +71926,7 @@
         <v>1369</v>
       </c>
       <c r="C596" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="D596" t="str">
         <f t="shared" si="9"/>
@@ -71939,7 +71941,7 @@
         <v>1371</v>
       </c>
       <c r="C597" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="D597" t="str">
         <f t="shared" si="9"/>
@@ -71954,7 +71956,7 @@
         <v>1373</v>
       </c>
       <c r="C598" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
       <c r="D598" t="str">
         <f t="shared" si="9"/>
@@ -72179,7 +72181,7 @@
         <v>1402</v>
       </c>
       <c r="C613" t="s">
-        <v>3692</v>
+        <v>3691</v>
       </c>
       <c r="D613" t="str">
         <f t="shared" si="9"/>
@@ -72194,7 +72196,7 @@
         <v>1404</v>
       </c>
       <c r="C614" t="s">
-        <v>3693</v>
+        <v>3692</v>
       </c>
       <c r="D614" t="str">
         <f t="shared" si="9"/>
@@ -72284,7 +72286,7 @@
         <v>1417</v>
       </c>
       <c r="C620" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="D620" t="str">
         <f t="shared" si="9"/>
@@ -72374,7 +72376,7 @@
         <v>1433</v>
       </c>
       <c r="C626" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="D626" t="str">
         <f t="shared" si="9"/>
@@ -72419,7 +72421,7 @@
         <v>1451</v>
       </c>
       <c r="C629" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="D629" t="str">
         <f t="shared" si="9"/>
@@ -72434,7 +72436,7 @@
         <v>1453</v>
       </c>
       <c r="C630" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="D630" t="str">
         <f t="shared" si="9"/>
@@ -72524,7 +72526,7 @@
         <v>1465</v>
       </c>
       <c r="C636" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
       <c r="D636" t="str">
         <f t="shared" si="9"/>
@@ -72539,7 +72541,7 @@
         <v>1467</v>
       </c>
       <c r="C637" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
       <c r="D637" t="str">
         <f t="shared" si="9"/>
@@ -72839,7 +72841,7 @@
         <v>1507</v>
       </c>
       <c r="C657" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="D657" t="str">
         <f t="shared" si="10"/>
@@ -72869,7 +72871,7 @@
         <v>1511</v>
       </c>
       <c r="C659" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="D659" t="str">
         <f t="shared" si="10"/>
@@ -73274,7 +73276,7 @@
         <v>1560</v>
       </c>
       <c r="C686" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="D686" t="str">
         <f t="shared" si="10"/>
@@ -73409,7 +73411,7 @@
         <v>1578</v>
       </c>
       <c r="C695" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
       <c r="D695" t="str">
         <f t="shared" si="10"/>
@@ -73424,7 +73426,7 @@
         <v>1580</v>
       </c>
       <c r="C696" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="D696" t="str">
         <f t="shared" si="10"/>
@@ -73499,7 +73501,7 @@
         <v>1590</v>
       </c>
       <c r="C701" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="D701" t="str">
         <f t="shared" si="10"/>
@@ -73604,7 +73606,7 @@
         <v>1606</v>
       </c>
       <c r="C708" s="3" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="D708" t="str">
         <f t="shared" si="11"/>
@@ -73769,7 +73771,7 @@
         <v>1627</v>
       </c>
       <c r="C719" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="D719" t="str">
         <f t="shared" si="11"/>
@@ -73859,7 +73861,7 @@
         <v>1639</v>
       </c>
       <c r="C725" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="D725" t="str">
         <f t="shared" si="11"/>
@@ -73919,7 +73921,7 @@
         <v>1647</v>
       </c>
       <c r="C729" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="D729" t="str">
         <f t="shared" si="11"/>
@@ -73934,7 +73936,7 @@
         <v>1649</v>
       </c>
       <c r="C730" s="5" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
       <c r="D730" t="str">
         <f t="shared" si="11"/>
@@ -74009,7 +74011,7 @@
         <v>1659</v>
       </c>
       <c r="C735" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="D735" t="str">
         <f t="shared" si="11"/>
@@ -74024,7 +74026,7 @@
         <v>1661</v>
       </c>
       <c r="C736" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="D736" t="str">
         <f t="shared" si="11"/>
@@ -74039,7 +74041,7 @@
         <v>1663</v>
       </c>
       <c r="C737" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="D737" t="str">
         <f t="shared" si="11"/>
@@ -74129,7 +74131,7 @@
         <v>1674</v>
       </c>
       <c r="C743" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="D743" t="str">
         <f t="shared" si="11"/>
@@ -74414,7 +74416,7 @@
         <v>1700</v>
       </c>
       <c r="C762" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="D762" t="str">
         <f t="shared" si="11"/>
@@ -74474,7 +74476,7 @@
         <v>1707</v>
       </c>
       <c r="C766" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="D766" t="str">
         <f t="shared" si="11"/>
@@ -74519,7 +74521,7 @@
         <v>1713</v>
       </c>
       <c r="C769" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="D769" t="str">
         <f t="shared" si="11"/>
@@ -74579,7 +74581,7 @@
         <v>1721</v>
       </c>
       <c r="C773" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="D773" t="str">
         <f t="shared" si="12"/>
@@ -74594,7 +74596,7 @@
         <v>1723</v>
       </c>
       <c r="C774" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="D774" t="str">
         <f t="shared" si="12"/>
@@ -74699,7 +74701,7 @@
         <v>1738</v>
       </c>
       <c r="C781" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="D781" t="str">
         <f t="shared" si="12"/>
@@ -74804,7 +74806,7 @@
         <v>1752</v>
       </c>
       <c r="C788" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="D788" t="str">
         <f t="shared" si="12"/>
@@ -74834,7 +74836,7 @@
         <v>1756</v>
       </c>
       <c r="C790" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D790" t="str">
         <f t="shared" si="12"/>
@@ -75089,7 +75091,7 @@
         <v>1793</v>
       </c>
       <c r="C807" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="D807" t="str">
         <f t="shared" si="12"/>
@@ -75104,7 +75106,7 @@
         <v>1795</v>
       </c>
       <c r="C808" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
       <c r="D808" t="str">
         <f t="shared" si="12"/>
@@ -75209,7 +75211,7 @@
         <v>38</v>
       </c>
       <c r="C815" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="D815" t="str">
         <f t="shared" si="12"/>
@@ -75299,7 +75301,7 @@
         <v>1746</v>
       </c>
       <c r="C821" s="3" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
       <c r="D821" t="str">
         <f t="shared" si="12"/>
@@ -75449,7 +75451,7 @@
         <v>1841</v>
       </c>
       <c r="C831" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
       <c r="D831" t="str">
         <f t="shared" si="12"/>
@@ -75464,7 +75466,7 @@
         <v>1843</v>
       </c>
       <c r="C832" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
       <c r="D832" t="str">
         <f t="shared" si="12"/>
@@ -75479,7 +75481,7 @@
         <v>1845</v>
       </c>
       <c r="C833" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="D833" t="str">
         <f t="shared" si="12"/>
@@ -75614,7 +75616,7 @@
         <v>1864</v>
       </c>
       <c r="C842" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="D842" t="str">
         <f t="shared" si="13"/>
@@ -75659,7 +75661,7 @@
         <v>1872</v>
       </c>
       <c r="C845" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="D845" t="str">
         <f t="shared" si="13"/>
@@ -75674,7 +75676,7 @@
         <v>1874</v>
       </c>
       <c r="C846" t="s">
-        <v>3694</v>
+        <v>3693</v>
       </c>
       <c r="D846" t="str">
         <f t="shared" si="13"/>
@@ -75719,7 +75721,7 @@
         <v>1880</v>
       </c>
       <c r="C849" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
       <c r="D849" t="str">
         <f t="shared" si="13"/>
@@ -75794,7 +75796,7 @@
         <v>14</v>
       </c>
       <c r="C854" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="D854" t="str">
         <f t="shared" si="13"/>
@@ -75824,7 +75826,7 @@
         <v>14</v>
       </c>
       <c r="C856" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="D856" t="str">
         <f t="shared" si="13"/>
@@ -75989,7 +75991,7 @@
         <v>1916</v>
       </c>
       <c r="C867" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="D867" t="str">
         <f t="shared" si="13"/>
@@ -76154,7 +76156,7 @@
         <v>16</v>
       </c>
       <c r="C878" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="D878" t="str">
         <f t="shared" si="13"/>
@@ -76289,7 +76291,7 @@
         <v>1956</v>
       </c>
       <c r="C887" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="D887" t="str">
         <f t="shared" si="13"/>
@@ -76304,7 +76306,7 @@
         <v>1958</v>
       </c>
       <c r="C888" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
       <c r="D888" t="str">
         <f t="shared" si="13"/>
@@ -76469,7 +76471,7 @@
         <v>1978</v>
       </c>
       <c r="C899" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="D899" t="str">
         <f t="shared" si="14"/>
@@ -76484,7 +76486,7 @@
         <v>1978</v>
       </c>
       <c r="C900" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="D900" t="str">
         <f t="shared" si="14"/>
@@ -76559,7 +76561,7 @@
         <v>1988</v>
       </c>
       <c r="C905" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
       <c r="D905" t="str">
         <f t="shared" si="14"/>
@@ -76589,7 +76591,7 @@
         <v>1992</v>
       </c>
       <c r="C907" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
       <c r="D907" t="str">
         <f t="shared" si="14"/>
@@ -76649,7 +76651,7 @@
         <v>2000</v>
       </c>
       <c r="C911" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="D911" t="str">
         <f t="shared" si="14"/>
@@ -76664,7 +76666,7 @@
         <v>2002</v>
       </c>
       <c r="C912" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="D912" t="str">
         <f t="shared" si="14"/>
@@ -76709,7 +76711,7 @@
         <v>2008</v>
       </c>
       <c r="C915" s="3" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
       <c r="D915" t="str">
         <f t="shared" si="14"/>
@@ -76784,7 +76786,7 @@
         <v>2018</v>
       </c>
       <c r="C920" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
       <c r="D920" t="str">
         <f t="shared" si="14"/>
@@ -76844,7 +76846,7 @@
         <v>2026</v>
       </c>
       <c r="C924" t="s">
-        <v>3681</v>
+        <v>3680</v>
       </c>
       <c r="D924" t="str">
         <f t="shared" si="14"/>
@@ -76874,7 +76876,7 @@
         <v>2030</v>
       </c>
       <c r="C926" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="D926" t="str">
         <f t="shared" si="14"/>
@@ -77474,7 +77476,7 @@
         <v>2127</v>
       </c>
       <c r="C966" s="2" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="D966" t="str">
         <f t="shared" si="15"/>
@@ -78014,7 +78016,7 @@
         <v>2002</v>
       </c>
       <c r="C1002" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="D1002" t="str">
         <f t="shared" si="15"/>
@@ -78269,7 +78271,7 @@
         <v>2211</v>
       </c>
       <c r="C1019" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
       <c r="D1019" t="str">
         <f t="shared" si="15"/>
@@ -78824,7 +78826,7 @@
         <v>2321</v>
       </c>
       <c r="C1056" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
       <c r="D1056" t="str">
         <f t="shared" si="16"/>
@@ -78914,7 +78916,7 @@
         <v>2332</v>
       </c>
       <c r="C1062" t="s">
-        <v>3685</v>
+        <v>3684</v>
       </c>
       <c r="D1062" t="str">
         <f t="shared" si="16"/>
@@ -78959,7 +78961,7 @@
         <v>2340</v>
       </c>
       <c r="C1065" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="D1065" t="str">
         <f t="shared" si="16"/>
@@ -79019,7 +79021,7 @@
         <v>95</v>
       </c>
       <c r="C1069" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="D1069" t="str">
         <f t="shared" si="16"/>
@@ -79109,7 +79111,7 @@
         <v>2359</v>
       </c>
       <c r="C1075" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="D1075" t="str">
         <f t="shared" si="16"/>
@@ -81059,7 +81061,7 @@
         <v>2598</v>
       </c>
       <c r="C1205" t="s">
-        <v>3688</v>
+        <v>3687</v>
       </c>
       <c r="D1205" t="str">
         <f t="shared" si="18"/>
@@ -81374,7 +81376,7 @@
         <v>3405</v>
       </c>
       <c r="C1226" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
       <c r="D1226" t="str">
         <f t="shared" si="19"/>
@@ -81404,7 +81406,7 @@
         <v>38</v>
       </c>
       <c r="C1228" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="D1228" t="str">
         <f t="shared" si="19"/>
@@ -81704,7 +81706,7 @@
         <v>3449</v>
       </c>
       <c r="C1248" t="s">
-        <v>3690</v>
+        <v>3689</v>
       </c>
       <c r="D1248" t="str">
         <f t="shared" si="19"/>
@@ -81719,7 +81721,7 @@
         <v>3474</v>
       </c>
       <c r="C1249" t="s">
-        <v>3691</v>
+        <v>3690</v>
       </c>
       <c r="D1249" t="str">
         <f t="shared" si="19"/>
@@ -81809,7 +81811,7 @@
         <v>3487</v>
       </c>
       <c r="C1255" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="D1255" t="str">
         <f t="shared" si="19"/>

</xml_diff>